<commit_message>
14.06. new extesion type 0x56 for max 4 temperature values per device
</commit_message>
<xml_diff>
--- a/stm32l4/Doc/DataFrames.xlsx
+++ b/stm32l4/Doc/DataFrames.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9700F171-BA58-4F14-887E-FD70F17AA775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0AF5B0-5C2D-4746-9736-AD15D13F5FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="4560" windowWidth="36200" windowHeight="14230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2660" windowWidth="36200" windowHeight="14230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PacketFormat" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
   <si>
     <t>Format of RFM12-Data Packets</t>
   </si>
@@ -414,19 +414,28 @@
     <t>Temp0[lo]</t>
   </si>
   <si>
-    <t>Temp2[7:0]</t>
-  </si>
-  <si>
-    <t>Temp4[7:0]</t>
-  </si>
-  <si>
-    <t>Temp1[7:0]</t>
-  </si>
-  <si>
-    <t>Temp3[7:0]</t>
-  </si>
-  <si>
-    <t>TempX[9:8]</t>
+    <t>CounterV2</t>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>Temp1[hi]</t>
+  </si>
+  <si>
+    <t>Temp1[lo]</t>
+  </si>
+  <si>
+    <t>Temp2[lo]</t>
+  </si>
+  <si>
+    <t>Temp2[hi]</t>
+  </si>
+  <si>
+    <t>Temp3[lo]</t>
+  </si>
+  <si>
+    <t>Temp3[hi]</t>
   </si>
 </sst>
 </file>
@@ -562,6 +571,9 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,9 +590,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -898,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:S42"/>
+  <dimension ref="B4:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21:U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,17 +933,17 @@
     <col min="18" max="18" width="21.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
@@ -982,7 +991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
@@ -1020,7 +1029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>6</v>
       </c>
@@ -1063,7 +1072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>7</v>
       </c>
@@ -1095,7 +1104,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>9</v>
       </c>
@@ -1111,7 +1120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="M16" s="2" t="s">
         <v>27</v>
       </c>
@@ -1139,8 +1148,14 @@
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="T16" s="2">
+        <v>16</v>
+      </c>
+      <c r="U16" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L17" t="s">
         <v>111</v>
       </c>
@@ -1162,7 +1177,7 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L18" t="s">
         <v>112</v>
       </c>
@@ -1186,284 +1201,302 @@
       </c>
       <c r="S18" s="1"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L19" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>123</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="H20" t="s">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="L20" t="s">
+        <v>118</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
         <v>126</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>127</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>124</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="O20" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="P20" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="R20" s="1" t="s">
+      <c r="P21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="S20" s="1"/>
-    </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="R21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6" t="s">
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="K22" s="6"/>
-      <c r="L22" s="6"/>
-      <c r="M22" s="5" t="s">
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="C23" s="3" t="s">
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="C24" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>95</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E24" t="s">
         <v>96</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
         <v>100</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>103</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="D24" t="s">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="D25" t="s">
         <v>97</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>98</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" t="s">
         <v>101</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>105</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="H25" t="s">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
         <v>106</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="2">
         <v>0</v>
       </c>
-      <c r="D30" s="2">
-        <f>C30+1</f>
+      <c r="D31" s="2">
+        <f>C31+1</f>
         <v>1</v>
       </c>
-      <c r="E30" s="2">
-        <f t="shared" ref="E30" si="5">D30+1</f>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31" si="5">D31+1</f>
         <v>2</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F31" s="2">
         <v>3</v>
       </c>
-      <c r="G30" s="2">
-        <f t="shared" ref="G30:H30" si="6">F30+1</f>
+      <c r="G31" s="2">
+        <f t="shared" ref="G31:H31" si="6">F31+1</f>
         <v>4</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H31" s="2">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J31" s="2">
         <v>6</v>
       </c>
-      <c r="K30" s="2">
-        <f t="shared" ref="K30" si="7">J30+1</f>
+      <c r="K31" s="2">
+        <f t="shared" ref="K31" si="7">J31+1</f>
         <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="J32" t="s">
-        <v>86</v>
-      </c>
-      <c r="K32" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="33" spans="3:13" x14ac:dyDescent="0.35">
       <c r="J33" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="J34" t="s">
         <v>87</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K34" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C34" s="3" t="s">
+    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C35" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>72</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>76</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>77</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>80</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="C35" t="s">
+    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
         <v>71</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>73</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F36" t="s">
         <v>78</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G36" t="s">
         <v>81</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H36" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="D36" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="3:13" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="D38" t="s">
         <v>75</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="J39" s="2">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="J40" s="2">
         <v>6</v>
       </c>
-      <c r="K39" s="2">
-        <f t="shared" ref="K39" si="8">J39+1</f>
+      <c r="K40" s="2">
+        <f t="shared" ref="K40" si="8">J40+1</f>
         <v>7</v>
       </c>
-      <c r="L39" s="2">
-        <f t="shared" ref="L39" si="9">K39+1</f>
+      <c r="L40" s="2">
+        <f t="shared" ref="L40" si="9">K40+1</f>
         <v>8</v>
       </c>
-      <c r="M39" s="2">
-        <f t="shared" ref="M39" si="10">L39+1</f>
+      <c r="M40" s="2">
+        <f t="shared" ref="M40" si="10">L40+1</f>
         <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.35">
-      <c r="J41" t="s">
-        <v>89</v>
-      </c>
-      <c r="K41" t="s">
-        <v>89</v>
-      </c>
-      <c r="L41" t="s">
-        <v>89</v>
-      </c>
-      <c r="M41" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="42" spans="3:13" x14ac:dyDescent="0.35">
       <c r="J42" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42" t="s">
+        <v>89</v>
+      </c>
+      <c r="L42" t="s">
+        <v>89</v>
+      </c>
+      <c r="M42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="J43" t="s">
         <v>93</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K43" t="s">
         <v>92</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L43" t="s">
         <v>91</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M43" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:O23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1655,10 +1688,10 @@
       <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="7"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
@@ -1667,49 +1700,49 @@
       <c r="D6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
-      <c r="AJ6" s="13"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="13"/>
-      <c r="AO6" s="13"/>
-      <c r="AP6" s="12" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AQ6" s="12"/>
+      <c r="AQ6" s="13"/>
     </row>
     <row r="8" spans="2:43" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
@@ -1718,50 +1751,50 @@
       <c r="C8">
         <v>29.59</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
-      <c r="Y8" s="9"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
-      <c r="AF8" s="9"/>
-      <c r="AG8" s="9"/>
-      <c r="AH8" s="9"/>
-      <c r="AI8" s="9"/>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
-      <c r="AM8" s="9"/>
-      <c r="AN8" s="9"/>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="8" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AQ8" s="8"/>
+      <c r="AQ8" s="9"/>
     </row>
     <row r="9" spans="2:43" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
@@ -1771,78 +1804,78 @@
         <v>66</v>
       </c>
       <c r="E9" s="14"/>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="10"/>
+      <c r="I9" s="11"/>
       <c r="J9" s="15" t="s">
         <v>47</v>
       </c>
       <c r="K9" s="15"/>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="9" t="s">
+      <c r="M9" s="7"/>
+      <c r="N9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="7" t="s">
+      <c r="O9" s="10"/>
+      <c r="P9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="13" t="s">
+      <c r="Q9" s="8"/>
+      <c r="R9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="9" t="s">
+      <c r="S9" s="7"/>
+      <c r="T9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="U9" s="9"/>
-      <c r="V9" s="7" t="s">
+      <c r="U9" s="10"/>
+      <c r="V9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="W9" s="7"/>
-      <c r="X9" s="13" t="s">
+      <c r="W9" s="8"/>
+      <c r="X9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="9" t="s">
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AA9" s="9"/>
-      <c r="AB9" s="7" t="s">
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="13" t="s">
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="9" t="s">
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AG9" s="9"/>
-      <c r="AH9" s="7" t="s">
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AI9" s="7"/>
-      <c r="AJ9" s="13" t="s">
+      <c r="AI9" s="8"/>
+      <c r="AJ9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="9" t="s">
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="AM9" s="9"/>
-      <c r="AN9" s="7" t="s">
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AO9" s="7"/>
+      <c r="AO9" s="8"/>
     </row>
     <row r="16" spans="2:43" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
@@ -1924,14 +1957,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="AH9:AI9"/>
-    <mergeCell ref="AJ9:AK9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="X9:Y9"/>
-    <mergeCell ref="AB9:AC9"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="AP8:AQ8"/>
     <mergeCell ref="AN9:AO9"/>
@@ -1948,6 +1973,14 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="AH9:AI9"/>
+    <mergeCell ref="AJ9:AK9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="AB9:AC9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>